<commit_message>
razor engine refacotor for dataconvert tool
</commit_message>
<xml_diff>
--- a/developWorkspace/CodeLibrary/CodeGenerator/addinCodeConverter3/dataConvertTools.xlsx
+++ b/developWorkspace/CodeLibrary/CodeGenerator/addinCodeConverter3/dataConvertTools.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xujingjiang\Source\Repos\developSupportToolls\developWorkspace\CodeLibrary\CodeGenerator\addinCodeConverter3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xujingjiang\Source\Repos\developSupportToolls\developWorkspace\bin\Debug\addins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D1821B-EA68-4909-B842-6D14CD0866B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDA3E35-FE49-4CE0-A68C-AF7C4381F5E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="113">
   <si>
     <t>Setting{}</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>DELETE:delete</t>
-  </si>
-  <si>
-    <t>*</t>
   </si>
   <si>
     <t>TOKEN</t>
@@ -689,32 +686,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <r>
-      <t>y</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.25"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>es</t>
-    </r>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>K</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>S</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>W</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>Key</t>
     <phoneticPr fontId="4"/>
   </si>
@@ -728,6 +699,22 @@
   </si>
   <si>
     <t>○</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>isK</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>isS</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>isW</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1209,6 +1196,9 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1224,9 +1214,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1510,7 +1497,7 @@
   <dimension ref="A1:CY196"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1"/>
@@ -1541,12 +1528,12 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="75" t="s">
-        <v>89</v>
+      <c r="D1" s="78" t="s">
+        <v>88</v>
       </c>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1563,13 +1550,13 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="67" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="X1" s="68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y1" s="68" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Z1" s="69"/>
       <c r="AA1" s="70"/>
@@ -1651,7 +1638,7 @@
     </row>
     <row r="2" spans="1:102" s="42" customFormat="1" ht="21">
       <c r="C2" s="43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="44"/>
       <c r="E2" s="45"/>
@@ -1662,7 +1649,7 @@
         <v>12</v>
       </c>
       <c r="Y2" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z2" s="51"/>
       <c r="AA2" s="63"/>
@@ -1673,11 +1660,11 @@
         <v>0</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="75" t="s">
-        <v>84</v>
+      <c r="D3" s="78" t="s">
+        <v>83</v>
       </c>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
       <c r="G3" s="39"/>
       <c r="H3" s="39"/>
       <c r="I3" s="1"/>
@@ -1686,13 +1673,13 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="W3" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="X3" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="X3" s="26" t="s">
-        <v>94</v>
-      </c>
       <c r="Y3" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Z3" s="27"/>
       <c r="AA3" s="64"/>
@@ -1710,24 +1697,24 @@
       <c r="G4" s="53"/>
       <c r="H4" s="54"/>
       <c r="I4" s="55"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
       <c r="L4" s="51"/>
-      <c r="N4" s="76" t="s">
-        <v>85</v>
+      <c r="N4" s="79" t="s">
+        <v>84</v>
       </c>
-      <c r="O4" s="76"/>
-      <c r="P4" s="76"/>
-      <c r="Q4" s="76"/>
-      <c r="R4" s="76"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="79"/>
       <c r="W4" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="X4" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="X4" s="27" t="s">
-        <v>96</v>
-      </c>
       <c r="Y4" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Z4" s="51"/>
       <c r="AA4" s="63"/>
@@ -1744,24 +1731,24 @@
       <c r="G5" s="56"/>
       <c r="H5" s="52"/>
       <c r="I5" s="57"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
       <c r="L5" s="26"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="76"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="76"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="79"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="65" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X5" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Y5" s="51"/>
       <c r="Z5" s="26"/>
@@ -1854,15 +1841,15 @@
       <c r="G6" s="56"/>
       <c r="H6" s="52"/>
       <c r="I6" s="57"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
       <c r="L6" s="26"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="76"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="76"/>
-      <c r="R6" s="76"/>
+      <c r="N6" s="79"/>
+      <c r="O6" s="79"/>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="79"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -1960,15 +1947,15 @@
       <c r="G7" s="56"/>
       <c r="H7" s="52"/>
       <c r="I7" s="57"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
       <c r="L7" s="26"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="76"/>
-      <c r="O7" s="76"/>
-      <c r="P7" s="76"/>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="76"/>
+      <c r="N7" s="79"/>
+      <c r="O7" s="79"/>
+      <c r="P7" s="79"/>
+      <c r="Q7" s="79"/>
+      <c r="R7" s="79"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
@@ -2066,15 +2053,15 @@
       <c r="G8" s="56"/>
       <c r="H8" s="52"/>
       <c r="I8" s="57"/>
-      <c r="J8" s="79"/>
-      <c r="K8" s="79"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
       <c r="L8" s="26"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="76"/>
-      <c r="O8" s="76"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="76"/>
+      <c r="N8" s="79"/>
+      <c r="O8" s="79"/>
+      <c r="P8" s="79"/>
+      <c r="Q8" s="79"/>
+      <c r="R8" s="79"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
@@ -2172,15 +2159,15 @@
       <c r="G9" s="58"/>
       <c r="H9" s="59"/>
       <c r="I9" s="60"/>
-      <c r="J9" s="79"/>
-      <c r="K9" s="79"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
       <c r="L9" s="26"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="76"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="76"/>
-      <c r="R9" s="76"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="79"/>
+      <c r="P9" s="79"/>
+      <c r="Q9" s="79"/>
+      <c r="R9" s="79"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
@@ -2375,10 +2362,10 @@
     <row r="11" spans="1:102" ht="18.75" customHeight="1">
       <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="1"/>
@@ -2796,12 +2783,12 @@
     <row r="15" spans="1:102" ht="20.25" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="39"/>
-      <c r="C15" s="74" t="s">
-        <v>86</v>
+      <c r="C15" s="77" t="s">
+        <v>85</v>
       </c>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -2809,13 +2796,13 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="74" t="s">
-        <v>87</v>
+      <c r="N15" s="77" t="s">
+        <v>86</v>
       </c>
-      <c r="O15" s="74"/>
-      <c r="P15" s="74"/>
-      <c r="Q15" s="74"/>
-      <c r="R15" s="74"/>
+      <c r="O15" s="77"/>
+      <c r="P15" s="77"/>
+      <c r="Q15" s="77"/>
+      <c r="R15" s="77"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
@@ -2905,23 +2892,23 @@
       <c r="A16" s="1"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
-      <c r="D16" s="77" t="s">
-        <v>88</v>
+      <c r="D16" s="80" t="s">
+        <v>87</v>
       </c>
-      <c r="E16" s="77"/>
-      <c r="F16" s="77"/>
-      <c r="G16" s="77"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="74"/>
-      <c r="O16" s="74"/>
-      <c r="P16" s="74"/>
-      <c r="Q16" s="74"/>
-      <c r="R16" s="74"/>
+      <c r="N16" s="77"/>
+      <c r="O16" s="77"/>
+      <c r="P16" s="77"/>
+      <c r="Q16" s="77"/>
+      <c r="R16" s="77"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
@@ -3018,13 +3005,13 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="39" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="K17" s="39" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="L17" s="39" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -3340,10 +3327,10 @@
       <c r="D20" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="73"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="77"/>
       <c r="I20" s="26"/>
       <c r="J20" s="26"/>
       <c r="K20" s="26"/>
@@ -3659,10 +3646,10 @@
       <c r="A23" s="1"/>
       <c r="B23" s="24"/>
       <c r="C23" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" s="71" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="26"/>
@@ -3788,13 +3775,13 @@
         <v>30</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="L24" s="15" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="M24" s="35" t="s">
         <v>31</v>
@@ -3904,43 +3891,43 @@
       <c r="B25" s="24"/>
       <c r="C25" s="3"/>
       <c r="D25" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="F25" s="6" t="s">
+      <c r="G25" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="H25" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="I25" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="J25" s="75" t="s">
+        <v>108</v>
+      </c>
+      <c r="K25" s="75" t="s">
+        <v>108</v>
+      </c>
+      <c r="L25" s="75" t="s">
+        <v>108</v>
+      </c>
+      <c r="M25" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="J25" s="80" t="s">
-        <v>113</v>
+      <c r="N25" s="75" t="s">
+        <v>108</v>
       </c>
-      <c r="K25" s="80" t="s">
-        <v>113</v>
+      <c r="O25" s="75" t="s">
+        <v>108</v>
       </c>
-      <c r="L25" s="80" t="s">
-        <v>113</v>
-      </c>
-      <c r="M25" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="N25" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="O25" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="P25" s="33" t="s">
-        <v>37</v>
+      <c r="P25" s="75" t="s">
+        <v>108</v>
       </c>
       <c r="Q25" s="32"/>
       <c r="R25" s="32"/>
@@ -4034,41 +4021,41 @@
       <c r="B26" s="24"/>
       <c r="C26" s="26"/>
       <c r="D26" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G26" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="I26" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I26" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="J26" s="6"/>
-      <c r="K26" s="80" t="s">
-        <v>113</v>
+      <c r="K26" s="75" t="s">
+        <v>108</v>
       </c>
       <c r="L26" s="6"/>
       <c r="M26" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
-      <c r="N26" s="33" t="s">
-        <v>37</v>
+      <c r="N26" s="75" t="s">
+        <v>108</v>
       </c>
-      <c r="O26" s="33" t="s">
-        <v>37</v>
+      <c r="O26" s="75" t="s">
+        <v>108</v>
       </c>
-      <c r="P26" s="33" t="s">
-        <v>37</v>
+      <c r="P26" s="75" t="s">
+        <v>108</v>
       </c>
       <c r="Q26" s="32"/>
-      <c r="R26" s="33" t="s">
-        <v>37</v>
+      <c r="R26" s="75" t="s">
+        <v>108</v>
       </c>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
@@ -4160,33 +4147,33 @@
       <c r="B27" s="24"/>
       <c r="C27" s="26"/>
       <c r="D27" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G27" s="6" t="s">
+      <c r="H27" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="I27" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I27" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="J27" s="6"/>
-      <c r="K27" s="80" t="s">
-        <v>113</v>
+      <c r="K27" s="75" t="s">
+        <v>108</v>
       </c>
       <c r="L27" s="6"/>
       <c r="M27" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
-      <c r="N27" s="33" t="s">
-        <v>37</v>
+      <c r="N27" s="75" t="s">
+        <v>108</v>
       </c>
       <c r="O27" s="33"/>
       <c r="P27" s="32"/>
@@ -4282,33 +4269,33 @@
       <c r="B28" s="24"/>
       <c r="C28" s="26"/>
       <c r="D28" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="62" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G28" s="14" t="s">
+      <c r="H28" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="I28" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="I28" s="14" t="s">
-        <v>57</v>
-      </c>
       <c r="J28" s="14"/>
-      <c r="K28" s="80" t="s">
-        <v>113</v>
+      <c r="K28" s="75" t="s">
+        <v>108</v>
       </c>
       <c r="L28" s="14"/>
       <c r="M28" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
-      <c r="N28" s="33" t="s">
-        <v>37</v>
+      <c r="N28" s="75" t="s">
+        <v>108</v>
       </c>
       <c r="O28" s="32"/>
       <c r="P28" s="32"/>
@@ -4404,33 +4391,33 @@
       <c r="B29" s="24"/>
       <c r="C29" s="28"/>
       <c r="D29" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="33" t="s">
+      <c r="F29" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="F29" s="33" t="s">
+      <c r="G29" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="33" t="s">
+      <c r="H29" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="H29" s="33" t="s">
+      <c r="I29" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="I29" s="33" t="s">
-        <v>63</v>
-      </c>
       <c r="J29" s="33"/>
-      <c r="K29" s="80" t="s">
-        <v>113</v>
+      <c r="K29" s="75" t="s">
+        <v>108</v>
       </c>
       <c r="L29" s="33"/>
       <c r="M29" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
-      <c r="N29" s="33" t="s">
-        <v>37</v>
+      <c r="N29" s="75" t="s">
+        <v>108</v>
       </c>
       <c r="O29" s="32"/>
       <c r="P29" s="32"/>
@@ -4526,31 +4513,31 @@
       <c r="B30" s="24"/>
       <c r="C30" s="37"/>
       <c r="D30" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="33" t="s">
+      <c r="F30" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="F30" s="33" t="s">
+      <c r="G30" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="G30" s="33" t="s">
+      <c r="H30" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="H30" s="33" t="s">
+      <c r="I30" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="I30" s="33" t="s">
-        <v>69</v>
-      </c>
       <c r="J30" s="33"/>
-      <c r="K30" s="80" t="s">
-        <v>113</v>
+      <c r="K30" s="75" t="s">
+        <v>108</v>
       </c>
       <c r="L30" s="33"/>
       <c r="M30" s="32"/>
-      <c r="N30" s="33" t="s">
-        <v>37</v>
+      <c r="N30" s="75" t="s">
+        <v>108</v>
       </c>
       <c r="O30" s="32"/>
       <c r="P30" s="32"/>
@@ -4646,24 +4633,24 @@
       <c r="B31" s="24"/>
       <c r="C31" s="26"/>
       <c r="D31" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E31" s="32"/>
       <c r="F31" s="33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G31" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="H31" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="H31" s="33" t="s">
+      <c r="I31" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="I31" s="33" t="s">
-        <v>73</v>
-      </c>
       <c r="J31" s="33"/>
-      <c r="K31" s="80" t="s">
-        <v>113</v>
+      <c r="K31" s="75" t="s">
+        <v>108</v>
       </c>
       <c r="L31" s="33"/>
       <c r="M31" s="32"/>
@@ -4762,24 +4749,24 @@
       <c r="B32" s="24"/>
       <c r="C32" s="26"/>
       <c r="D32" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E32" s="32"/>
       <c r="F32" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G32" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="H32" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="H32" s="33" t="s">
+      <c r="I32" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="I32" s="33" t="s">
-        <v>77</v>
-      </c>
       <c r="J32" s="33"/>
-      <c r="K32" s="80" t="s">
-        <v>113</v>
+      <c r="K32" s="75" t="s">
+        <v>108</v>
       </c>
       <c r="L32" s="33"/>
       <c r="M32" s="32"/>
@@ -4878,24 +4865,24 @@
       <c r="B33" s="24"/>
       <c r="C33" s="26"/>
       <c r="D33" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E33" s="32"/>
       <c r="F33" s="33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G33" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H33" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="I33" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="I33" s="33" t="s">
-        <v>80</v>
-      </c>
       <c r="J33" s="33"/>
-      <c r="K33" s="80" t="s">
-        <v>113</v>
+      <c r="K33" s="75" t="s">
+        <v>108</v>
       </c>
       <c r="L33" s="33"/>
       <c r="M33" s="32"/>

</xml_diff>